<commit_message>
adding accuracy metrics and measures of fit for msa model
</commit_message>
<xml_diff>
--- a/output/msa_df_accuracy_table.xlsx
+++ b/output/msa_df_accuracy_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\inflation_cr_expansion\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC59AB6-731C-4B67-A9B1-D540722B9069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23005966-E9F3-4913-8279-F3A3002DA861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msa_df_flag" sheetId="1" r:id="rId1"/>
@@ -1019,7 +1019,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A54" sqref="A54"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8089,7 +8089,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B37:U52 B54:U56">
+  <conditionalFormatting sqref="B37:U52 B54:U56 W54:W55">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$B$40</formula>
     </cfRule>

</xml_diff>

<commit_message>
writing and accuracy metrics
</commit_message>
<xml_diff>
--- a/output/msa_df_accuracy_table.xlsx
+++ b/output/msa_df_accuracy_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\inflation_cr_expansion\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4C9CF0-17B2-444D-B7E5-F8F058B90D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9189B0-D701-4194-9635-882B53AFA77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
   <si>
     <t>Atlanta</t>
   </si>
@@ -145,12 +145,6 @@
   </si>
   <si>
     <t>CR end to end (end 05 to end 06)</t>
-  </si>
-  <si>
-    <t>Strategy Outperformance</t>
-  </si>
-  <si>
-    <t>StartingCR</t>
   </si>
 </sst>
 </file>
@@ -716,7 +710,27 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -785,13 +799,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Strat Performs better on lower</a:t>
+              <a:t>Strat out(under) performance vs Buy &amp; Hold</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> CRs</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -827,824 +836,174 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>msa_df_flag!$A$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>strat out(under) performance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{041CB1DF-C10F-461E-B321-0E1118669F05}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{A9D0F9B3-7F7F-4603-B4C6-E9FC0ED85C18}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{1A064A31-DF05-43BD-AC2F-62B21C3239BF}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{B3BC7273-E041-49E2-9F4F-87F52806DB70}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000F-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{DABBAE39-2F0A-41E7-B7F3-AED0979400BD}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000010-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{1F92868F-C0C8-40C9-BEDA-42C50C3E7C96}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000011-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="11"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{3AFC2BD0-8182-446F-8EFC-ECC58A5A0F83}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000012-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="12"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="13"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{ECA15076-C696-48AE-AE79-6E9836A816E8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000013-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="14"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{FFDCDB87-02CF-4C85-B429-9CF8156B2FBC}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000014-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="15"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-9.9886480718763188E-2"/>
-                  <c:y val="-2.7777777777777863E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{5E728B3E-EFE3-408C-8206-BA08D500A29D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="16"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{B84DC3DE-AB00-4BD4-BB45-8A02FA64DFF2}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000015-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="17"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="18"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="1.8518518518518517E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{FE487A75-C8CD-4CC1-9F91-FDFAE925A5B0}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="19"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-1E51-4C8D-B283-3682A48D444D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showDataLabelsRange val="1"/>
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.8204813602039328E-2"/>
-                  <c:y val="-0.51470290172061828"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>msa_df_flag!$Y$70:$Y$89</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>SanDiego</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Miami</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NewYork</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Phoenix</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Detroit</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SanFrancisco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tampa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>LosAngeles</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dallas</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Denver</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>StLouis</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Baltimore</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Chicago</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Boston</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Minneapolis</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Seattle</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Atlanta</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Philadelphia</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>WashingtonDC</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Houston</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>msa_df_flag!$X$73:$X$92</c:f>
+              <c:f>msa_df_flag!$X$70:$X$89</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>6.56853648392203E-2</c:v>
+                  <c:v>1.8690297687607345</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8234567197658002E-2</c:v>
+                  <c:v>1.635966844972792</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4366622098576104E-2</c:v>
+                  <c:v>1.075708759111635</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.44981918732635E-2</c:v>
+                  <c:v>0.80336873602153713</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6130509136852006E-2</c:v>
+                  <c:v>0.63997393592636742</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6590900744514998E-2</c:v>
+                  <c:v>0.39052887397196256</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4546459226739294E-2</c:v>
+                  <c:v>0.37071626444984029</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.14931804494124E-2</c:v>
+                  <c:v>0.35948881871059912</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4218996551731402E-2</c:v>
+                  <c:v>0.35906272042060583</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1021976384384398E-2</c:v>
+                  <c:v>0.26674142688427094</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.44199395766646E-2</c:v>
+                  <c:v>0.1241318922593222</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.6300580220185102E-2</c:v>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>-7.4171418459878957E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.4974313343064097E-2</c:v>
+                  <c:v>-8.2369753394651468E-2</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.7788216139723701E-2</c:v>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>-8.4034089348028917E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.7407207633789097E-2</c:v>
+                  <c:v>-0.19068719018436686</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.9381859630104601E-2</c:v>
+                  <c:v>-0.20195623668708473</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.6465367791983002E-2</c:v>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>-0.25935693250475655</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.7071548821548796E-2</c:v>
+                  <c:v>-0.3754592711514928</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.3319946257295104E-2</c:v>
+                  <c:v>-0.42887445408766689</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.7079610448183798E-2</c:v>
+                  <c:v>-0.46140809794129778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>msa_df_flag!$Y$73:$Y$92</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>-0.15144863288279109</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.11827812366767798</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-7.4003061805737347E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.10728422065755572</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.56332807541223162</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.51192642756535567</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.92576845097068139</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.45350243685347147</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.49137770522605151</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7425550758754325</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.18817527234182485</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.74775927556761368</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.29973693978419291</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.4193582215655791</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.7682790693358452</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.49804890930928658</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-2.0006187760486904E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.64389593755008345</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.46418707052483588</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-0.29441348873434547</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:datalabelsRange>
-                <c15:f>msa_df_flag!$W$73:$W$92</c15:f>
-                <c15:dlblRangeCache>
-                  <c:ptCount val="20"/>
-                  <c:pt idx="0">
-                    <c:v>Atlanta</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Baltimore</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Boston</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Chicago</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Dallas</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Denver</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Detroit</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Houston</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>LosAngeles</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Miami</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Minneapolis</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>NewYork</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Philadelphia</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Phoenix</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>SanDiego</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>SanFrancisco</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Seattle</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>StLouis</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Tampa</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>WashingtonDC</c:v>
-                  </c:pt>
-                </c15:dlblRangeCache>
-              </c15:datalabelsRange>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7E75-43EE-B675-A98C6975117F}"/>
+              <c16:uniqueId val="{00000000-555D-4E24-8AA1-8398134B6C2C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1656,110 +1015,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1989464688"/>
-        <c:axId val="1989465520"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1989464688"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1748760240"/>
+        <c:axId val="1748761488"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1748760240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="4.0000000000000008E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>MSA's starting</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Cap Rate</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.40976462445567108"/>
-              <c:y val="0.90645815106445027"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1786,12 +1064,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1989465520"/>
+        <c:crossAx val="1748761488"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="1989465520"/>
+        <c:axId val="1748761488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,75 +1092,14 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Strat Outperformance vs Buy and Hold</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1903,9 +1123,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1989464688"/>
+        <c:crossAx val="1748760240"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2000,7 +1220,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2027,8 +1247,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2129,7 +1349,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2161,10 +1381,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2204,23 +1424,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2325,8 +1544,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2458,20 +1677,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2485,17 +1703,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2519,29 +1726,27 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>309996</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E83B2A40-7B3C-4F9E-879C-2B833243D4AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03B61020-BC36-43F7-A3E2-05DCD649BD2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2855,13 +2060,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y109"/>
+  <dimension ref="A1:Y114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S79" sqref="S79"/>
+      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7519,20 +6724,35 @@
       <c r="U69" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="X69" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
+      <c r="X70" s="1">
+        <v>1.8690297687607345</v>
+      </c>
+      <c r="Y70" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
+      <c r="X71" s="1">
+        <v>1.635966844972792</v>
+      </c>
+      <c r="Y71" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
-      <c r="X72" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y72" t="s">
-        <v>38</v>
+      <c r="X72" s="1">
+        <v>1.075708759111635</v>
+      </c>
+      <c r="Y72" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
@@ -7599,14 +6819,11 @@
       <c r="U73" t="s">
         <v>18</v>
       </c>
-      <c r="W73" t="s">
-        <v>0</v>
-      </c>
       <c r="X73" s="1">
-        <v>6.56853648392203E-2</v>
-      </c>
-      <c r="Y73" s="1">
-        <v>-0.15144863288279109</v>
+        <v>0.80336873602153713</v>
+      </c>
+      <c r="Y73" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
@@ -7673,14 +6890,11 @@
       <c r="U74" s="1">
         <v>5.7079610448183798E-2</v>
       </c>
-      <c r="W74" t="s">
-        <v>1</v>
-      </c>
       <c r="X74" s="1">
-        <v>5.8234567197658002E-2</v>
-      </c>
-      <c r="Y74" s="1">
-        <v>0.11827812366767798</v>
+        <v>0.63997393592636742</v>
+      </c>
+      <c r="Y74" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
@@ -7747,14 +6961,11 @@
       <c r="U75" s="1">
         <v>5.9893916237402103E-2</v>
       </c>
-      <c r="W75" t="s">
-        <v>2</v>
-      </c>
       <c r="X75" s="1">
-        <v>6.4366622098576104E-2</v>
-      </c>
-      <c r="Y75" s="1">
-        <v>-7.4003061805737347E-2</v>
+        <v>0.39052887397196256</v>
+      </c>
+      <c r="Y75" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
@@ -7821,14 +7032,11 @@
       <c r="U76" s="1">
         <v>5.6550714743074902E-2</v>
       </c>
-      <c r="W76" t="s">
-        <v>3</v>
-      </c>
       <c r="X76" s="1">
-        <v>6.44981918732635E-2</v>
-      </c>
-      <c r="Y76" s="1">
-        <v>-0.10728422065755572</v>
+        <v>0.37071626444984029</v>
+      </c>
+      <c r="Y76" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
@@ -7895,14 +7103,11 @@
       <c r="U77" s="1">
         <v>5.8980217508993397E-2</v>
       </c>
-      <c r="W77" t="s">
-        <v>4</v>
-      </c>
       <c r="X77" s="1">
-        <v>6.6130509136852006E-2</v>
-      </c>
-      <c r="Y77" s="1">
-        <v>0.56332807541223162</v>
+        <v>0.35948881871059912</v>
+      </c>
+      <c r="Y77" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
@@ -7969,14 +7174,11 @@
       <c r="U78" s="1">
         <v>6.6536825836332095E-2</v>
       </c>
-      <c r="W78" t="s">
-        <v>5</v>
-      </c>
       <c r="X78" s="1">
-        <v>5.6590900744514998E-2</v>
-      </c>
-      <c r="Y78" s="1">
-        <v>0.51192642756535567</v>
+        <v>0.35906272042060583</v>
+      </c>
+      <c r="Y78" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
@@ -8043,14 +7245,11 @@
       <c r="U79" s="1">
         <v>6.17983841921989E-2</v>
       </c>
-      <c r="W79" t="s">
-        <v>19</v>
-      </c>
       <c r="X79" s="1">
-        <v>6.4546459226739294E-2</v>
-      </c>
-      <c r="Y79" s="1">
-        <v>0.92576845097068139</v>
+        <v>0.26674142688427094</v>
+      </c>
+      <c r="Y79" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
@@ -8117,14 +7316,11 @@
       <c r="U80" s="1">
         <v>5.8613415713973598E-2</v>
       </c>
-      <c r="W80" t="s">
-        <v>6</v>
-      </c>
       <c r="X80" s="1">
-        <v>7.14931804494124E-2</v>
-      </c>
-      <c r="Y80" s="1">
-        <v>-0.45350243685347147</v>
+        <v>0.1241318922593222</v>
+      </c>
+      <c r="Y80" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
@@ -8191,14 +7387,11 @@
       <c r="U81" s="1">
         <v>5.6885440454410602E-2</v>
       </c>
-      <c r="W81" t="s">
-        <v>7</v>
-      </c>
-      <c r="X81" s="1">
-        <v>5.4218996551731402E-2</v>
-      </c>
-      <c r="Y81" s="1">
-        <v>0.49137770522605151</v>
+      <c r="X81">
+        <v>-7.4171418459878957E-2</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
@@ -8265,14 +7458,11 @@
       <c r="U82" s="1">
         <v>5.6753917715180499E-2</v>
       </c>
-      <c r="W82" t="s">
-        <v>8</v>
-      </c>
       <c r="X82" s="1">
-        <v>6.1021976384384398E-2</v>
-      </c>
-      <c r="Y82" s="1">
-        <v>1.7425550758754325</v>
+        <v>-8.2369753394651468E-2</v>
+      </c>
+      <c r="Y82" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
@@ -8339,14 +7529,11 @@
       <c r="U83" s="1">
         <v>5.60952170186916E-2</v>
       </c>
-      <c r="W83" t="s">
-        <v>9</v>
-      </c>
-      <c r="X83" s="1">
-        <v>6.44199395766646E-2</v>
-      </c>
-      <c r="Y83" s="1">
-        <v>-0.18817527234182485</v>
+      <c r="X83">
+        <v>-8.4034089348028917E-2</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
@@ -8413,14 +7600,11 @@
       <c r="U84" s="1">
         <v>5.4728025813493897E-2</v>
       </c>
-      <c r="W84" t="s">
-        <v>10</v>
-      </c>
       <c r="X84" s="1">
-        <v>5.6300580220185102E-2</v>
-      </c>
-      <c r="Y84" s="1">
-        <v>0.74775927556761368</v>
+        <v>-0.19068719018436686</v>
+      </c>
+      <c r="Y84" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
@@ -8487,14 +7671,11 @@
       <c r="U85" s="1">
         <v>5.36783642779926E-2</v>
       </c>
-      <c r="W85" t="s">
-        <v>11</v>
-      </c>
       <c r="X85" s="1">
-        <v>6.4974313343064097E-2</v>
-      </c>
-      <c r="Y85" s="1">
-        <v>-0.29973693978419291</v>
+        <v>-0.20195623668708473</v>
+      </c>
+      <c r="Y85" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
@@ -8561,14 +7742,11 @@
       <c r="U86" s="1">
         <v>5.3389030754752001E-2</v>
       </c>
-      <c r="W86" t="s">
-        <v>12</v>
-      </c>
-      <c r="X86" s="1">
-        <v>5.7788216139723701E-2</v>
-      </c>
-      <c r="Y86" s="1">
-        <v>1.4193582215655791</v>
+      <c r="X86">
+        <v>-0.25935693250475655</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
@@ -8635,14 +7813,11 @@
       <c r="U87" s="1">
         <v>5.2957804018772703E-2</v>
       </c>
-      <c r="W87" t="s">
-        <v>13</v>
-      </c>
       <c r="X87" s="1">
-        <v>4.7407207633789097E-2</v>
-      </c>
-      <c r="Y87" s="1">
-        <v>3.7682790693358452</v>
+        <v>-0.3754592711514928</v>
+      </c>
+      <c r="Y87" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
@@ -8709,14 +7884,11 @@
       <c r="U88" s="1">
         <v>5.3001447081666E-2</v>
       </c>
-      <c r="W88" t="s">
-        <v>14</v>
-      </c>
       <c r="X88" s="1">
-        <v>4.9381859630104601E-2</v>
-      </c>
-      <c r="Y88" s="1">
-        <v>0.49804890930928658</v>
+        <v>-0.42887445408766689</v>
+      </c>
+      <c r="Y88" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
@@ -8783,14 +7955,11 @@
       <c r="U89" s="1">
         <v>4.8790101872607801E-2</v>
       </c>
-      <c r="W89" t="s">
-        <v>15</v>
-      </c>
       <c r="X89" s="1">
-        <v>5.6465367791983002E-2</v>
-      </c>
-      <c r="Y89" s="1">
-        <v>-2.0006187760486904E-2</v>
+        <v>-0.46140809794129778</v>
+      </c>
+      <c r="Y89" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
@@ -8857,26 +8026,12 @@
       <c r="U90" s="1">
         <v>4.6838490123922903E-2</v>
       </c>
-      <c r="W90" t="s">
-        <v>16</v>
-      </c>
-      <c r="X90" s="1">
-        <v>6.7071548821548796E-2</v>
-      </c>
-      <c r="Y90" s="1">
-        <v>0.64389593755008345</v>
-      </c>
+      <c r="X90" s="1"/>
+      <c r="Y90" s="1"/>
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="W91" t="s">
-        <v>17</v>
-      </c>
-      <c r="X91" s="1">
-        <v>6.3319946257295104E-2</v>
-      </c>
-      <c r="Y91" s="1">
-        <v>0.46418707052483588</v>
-      </c>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
@@ -8942,15 +8097,8 @@
       <c r="U92" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W92" t="s">
-        <v>18</v>
-      </c>
-      <c r="X92" s="1">
-        <v>5.7079610448183798E-2</v>
-      </c>
-      <c r="Y92" s="1">
-        <v>-0.29441348873434547</v>
-      </c>
+      <c r="X92" s="1"/>
+      <c r="Y92" s="1"/>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
@@ -9206,6 +8354,8 @@
         <f t="shared" si="30"/>
         <v>2.4295027659184953E-3</v>
       </c>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
@@ -9291,8 +8441,10 @@
         <f t="shared" si="31"/>
         <v>7.5566083273386972E-3</v>
       </c>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>2009</v>
       </c>
@@ -9376,8 +8528,10 @@
         <f t="shared" si="32"/>
         <v>-4.7384416441331942E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X97" s="1"/>
+      <c r="Y97" s="1"/>
+    </row>
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>2010</v>
       </c>
@@ -9461,8 +8615,10 @@
         <f t="shared" si="33"/>
         <v>-3.1849684782253029E-3</v>
       </c>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X98" s="1"/>
+      <c r="Y98" s="1"/>
+    </row>
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>2011</v>
       </c>
@@ -9546,8 +8702,10 @@
         <f t="shared" si="34"/>
         <v>-1.7279752595629957E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X99" s="1"/>
+      <c r="Y99" s="1"/>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>2012</v>
       </c>
@@ -9631,8 +8789,10 @@
         <f t="shared" si="35"/>
         <v>-1.3152273923010271E-4</v>
       </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X100" s="1"/>
+      <c r="Y100" s="1"/>
+    </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>2013</v>
       </c>
@@ -9716,8 +8876,10 @@
         <f t="shared" si="36"/>
         <v>-6.5870069648889945E-4</v>
       </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+    </row>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>2014</v>
       </c>
@@ -9801,8 +8963,10 @@
         <f t="shared" si="37"/>
         <v>-1.3671912051977028E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X102" s="1"/>
+      <c r="Y102" s="1"/>
+    </row>
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>2015</v>
       </c>
@@ -9886,8 +9050,10 @@
         <f t="shared" si="38"/>
         <v>-1.0496615355012964E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X103" s="1"/>
+      <c r="Y103" s="1"/>
+    </row>
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>2016</v>
       </c>
@@ -9971,8 +9137,10 @@
         <f t="shared" si="39"/>
         <v>-2.8933352324059941E-4</v>
       </c>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X104" s="1"/>
+      <c r="Y104" s="1"/>
+    </row>
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>2017</v>
       </c>
@@ -10056,8 +9224,10 @@
         <f t="shared" si="40"/>
         <v>-4.3122673597929817E-4</v>
       </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+    </row>
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>2018</v>
       </c>
@@ -10141,8 +9311,10 @@
         <f t="shared" si="41"/>
         <v>4.3643062893297668E-5</v>
       </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X106" s="1"/>
+      <c r="Y106" s="1"/>
+    </row>
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>2019</v>
       </c>
@@ -10226,8 +9398,10 @@
         <f t="shared" si="42"/>
         <v>-4.2113452090581996E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X107" s="1"/>
+      <c r="Y107" s="1"/>
+    </row>
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>2020</v>
       </c>
@@ -10311,8 +9485,10 @@
         <f t="shared" si="43"/>
         <v>-1.9516117486848977E-3</v>
       </c>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X108" s="1"/>
+      <c r="Y108" s="1"/>
+    </row>
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -10334,14 +9510,51 @@
       <c r="S109" s="6"/>
       <c r="T109" s="6"/>
       <c r="U109" s="6"/>
+      <c r="X109" s="1"/>
+      <c r="Y109" s="1"/>
+    </row>
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X110" s="1"/>
+      <c r="Y110" s="1"/>
+    </row>
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X111" s="1"/>
+      <c r="Y111" s="1"/>
+    </row>
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X112" s="1"/>
+      <c r="Y112" s="1"/>
+    </row>
+    <row r="113" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X113" s="1"/>
+      <c r="Y113" s="1"/>
+    </row>
+    <row r="114" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X114" s="1"/>
+      <c r="Y114" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="X70:Y89">
+    <sortCondition descending="1" ref="X70:X89"/>
+  </sortState>
   <conditionalFormatting sqref="B39:U53">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"True Negative"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"True Positive"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:V67">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>